<commit_message>
vault backup: 2025-02-13 19:36:51
</commit_message>
<xml_diff>
--- a/de/fpu/include_f16div/radix4_srt_div.xlsx
+++ b/de/fpu/include_f16div/radix4_srt_div.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\obs\hw\fpu\include_f16div\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\obs\de\fpu\include_f16div\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D1917BD-8A05-49F1-B9E4-5336261C5C4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E65939F8-29A4-48AA-96D9-2EC4445EDD44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="29760" windowHeight="17496" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="29676" windowHeight="17496" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="div_srt" sheetId="1" r:id="rId1"/>
@@ -26931,6 +26931,50 @@
             <a:schemeClr val="accent1"/>
           </a:solidFill>
         </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>402338</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>46383</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>509125</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>4152</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{23A93CFD-E273-78CE-721A-08C90442CA09}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10997451" y="231913"/>
+          <a:ext cx="3764387" cy="2555196"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -37697,7 +37741,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
@@ -37987,8 +38031,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:AQ30"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -39412,7 +39456,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:AQ30"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView topLeftCell="B6" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
@@ -40800,8 +40844,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:AQ30"/>
   <sheetViews>
-    <sheetView topLeftCell="B60" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView topLeftCell="A3" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="Q23" sqref="Q23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -41858,7 +41902,7 @@
         <v>20.000000000000004</v>
       </c>
       <c r="Q23" s="10">
-        <f t="shared" si="12"/>
+        <f>SUM(Q$4*$H23*(2^$B$8)-$W$23)</f>
         <v>21.333333333333336</v>
       </c>
       <c r="W23">
@@ -43602,7 +43646,7 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:AQ30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+    <sheetView topLeftCell="A15" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
       <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>

</xml_diff>